<commit_message>
add datasets grouped by year To better understand how prosecution of crimes differed between George Gascon (2018-2019) and Chesa Boudin (2020-2021), we are dividing the dataset into a subset from 2018-2019 and 2020-2021. I've also added a chart to the file for the full dataset BY YEAR showing how the rate of dismissals for each incident type and the average CJ and SP terms for each incident type differed between the two periods.
</commit_message>
<xml_diff>
--- a/output files/MORE DETAILED SUMMARY BY Incident Subcategory.xlsx
+++ b/output files/MORE DETAILED SUMMARY BY Incident Subcategory.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5687" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5682" uniqueCount="384">
   <si>
     <t>Fraction missing values</t>
   </si>
@@ -2285,7 +2285,7 @@
         <v>129</v>
       </c>
       <c r="G29">
-        <v>1217</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="30" spans="1:14">
@@ -2306,7 +2306,7 @@
         <v>129</v>
       </c>
       <c r="G30">
-        <v>651</v>
+        <v>610</v>
       </c>
     </row>
     <row r="31" spans="1:14">
@@ -2327,7 +2327,7 @@
         <v>130</v>
       </c>
       <c r="G31">
-        <v>722</v>
+        <v>680</v>
       </c>
     </row>
     <row r="32" spans="1:14">
@@ -2336,7 +2336,7 @@
         <v>106</v>
       </c>
       <c r="C32">
-        <v>0.8403465346534653</v>
+        <v>0.8137376237623762</v>
       </c>
       <c r="D32" t="s">
         <v>113</v>
@@ -2345,7 +2345,7 @@
         <v>3</v>
       </c>
       <c r="H32">
-        <v>207513428.7790698</v>
+        <v>177868653.2392026</v>
       </c>
       <c r="I32">
         <v>0</v>
@@ -2363,7 +2363,7 @@
         <v>17748900625</v>
       </c>
       <c r="N32">
-        <v>1906342738.28757</v>
+        <v>1765938648.58772</v>
       </c>
     </row>
     <row r="33" spans="1:14">
@@ -2423,7 +2423,7 @@
         <v>0</v>
       </c>
       <c r="G35">
-        <v>1371</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="36" spans="1:14">
@@ -3136,7 +3136,7 @@
         <v>129</v>
       </c>
       <c r="G63">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="64" spans="1:13">
@@ -3157,7 +3157,7 @@
         <v>129</v>
       </c>
       <c r="G64">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="65" spans="1:14">
@@ -3178,7 +3178,7 @@
         <v>130</v>
       </c>
       <c r="G65">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="66" spans="1:14">
@@ -3187,7 +3187,7 @@
         <v>106</v>
       </c>
       <c r="C66">
-        <v>0.9369747899159664</v>
+        <v>0.9327731092436975</v>
       </c>
       <c r="D66" t="s">
         <v>113</v>
@@ -3274,7 +3274,7 @@
         <v>0</v>
       </c>
       <c r="G69">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="70" spans="1:14">
@@ -4802,7 +4802,7 @@
         <v>129</v>
       </c>
       <c r="G131">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="132" spans="1:14">
@@ -4823,7 +4823,7 @@
         <v>129</v>
       </c>
       <c r="G132">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="133" spans="1:14">
@@ -4844,7 +4844,7 @@
         <v>130</v>
       </c>
       <c r="G133">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="134" spans="1:14">
@@ -4853,7 +4853,7 @@
         <v>106</v>
       </c>
       <c r="C134">
-        <v>0.8733205374280231</v>
+        <v>0.8675623800383877</v>
       </c>
       <c r="D134" t="s">
         <v>113</v>
@@ -4940,7 +4940,7 @@
         <v>0</v>
       </c>
       <c r="G137">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="138" spans="1:14">
@@ -5653,7 +5653,7 @@
         <v>129</v>
       </c>
       <c r="G165">
-        <v>289</v>
+        <v>284</v>
       </c>
     </row>
     <row r="166" spans="1:14">
@@ -5668,13 +5668,13 @@
         <v>111</v>
       </c>
       <c r="E166">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F166" t="s">
         <v>129</v>
       </c>
       <c r="G166">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="167" spans="1:14">
@@ -5695,7 +5695,7 @@
         <v>130</v>
       </c>
       <c r="G167">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="168" spans="1:14">
@@ -5704,7 +5704,7 @@
         <v>106</v>
       </c>
       <c r="C168">
-        <v>0.8720626631853786</v>
+        <v>0.8590078328981723</v>
       </c>
       <c r="D168" t="s">
         <v>113</v>
@@ -5713,7 +5713,7 @@
         <v>3</v>
       </c>
       <c r="H168">
-        <v>362387860.1190476</v>
+        <v>328833428.6265432</v>
       </c>
       <c r="I168">
         <v>0</v>
@@ -5731,7 +5731,7 @@
         <v>17748900625</v>
       </c>
       <c r="N168">
-        <v>2535533375.768227</v>
+        <v>2415298888.47385</v>
       </c>
     </row>
     <row r="169" spans="1:14">
@@ -5791,7 +5791,7 @@
         <v>0</v>
       </c>
       <c r="G171">
-        <v>336</v>
+        <v>331</v>
       </c>
     </row>
     <row r="172" spans="1:14">
@@ -6504,7 +6504,7 @@
         <v>129</v>
       </c>
       <c r="G199">
-        <v>843</v>
+        <v>824</v>
       </c>
     </row>
     <row r="200" spans="1:14">
@@ -6525,7 +6525,7 @@
         <v>129</v>
       </c>
       <c r="G200">
-        <v>494</v>
+        <v>475</v>
       </c>
     </row>
     <row r="201" spans="1:14">
@@ -6546,7 +6546,7 @@
         <v>130</v>
       </c>
       <c r="G201">
-        <v>542</v>
+        <v>523</v>
       </c>
     </row>
     <row r="202" spans="1:14">
@@ -6555,7 +6555,7 @@
         <v>106</v>
       </c>
       <c r="C202">
-        <v>0.9083820662768031</v>
+        <v>0.8898635477582846</v>
       </c>
       <c r="D202" t="s">
         <v>113</v>
@@ -6564,7 +6564,7 @@
         <v>2</v>
       </c>
       <c r="H202">
-        <v>15734840.97960993</v>
+        <v>13089159.75294985</v>
       </c>
       <c r="I202">
         <v>0</v>
@@ -6582,7 +6582,7 @@
         <v>739537526.0416666</v>
       </c>
       <c r="N202">
-        <v>107291107.0734947</v>
+        <v>97946398.20568845</v>
       </c>
     </row>
     <row r="203" spans="1:14">
@@ -6642,7 +6642,7 @@
         <v>0</v>
       </c>
       <c r="G205">
-        <v>934</v>
+        <v>915</v>
       </c>
     </row>
     <row r="206" spans="1:14">
@@ -7355,7 +7355,7 @@
         <v>129</v>
       </c>
       <c r="G233">
-        <v>630</v>
+        <v>615</v>
       </c>
     </row>
     <row r="234" spans="1:14">
@@ -7376,7 +7376,7 @@
         <v>129</v>
       </c>
       <c r="G234">
-        <v>374</v>
+        <v>359</v>
       </c>
     </row>
     <row r="235" spans="1:14">
@@ -7397,7 +7397,7 @@
         <v>130</v>
       </c>
       <c r="G235">
-        <v>386</v>
+        <v>371</v>
       </c>
     </row>
     <row r="236" spans="1:14">
@@ -7406,7 +7406,7 @@
         <v>106</v>
       </c>
       <c r="C236">
-        <v>0.8746958637469586</v>
+        <v>0.8564476885644768</v>
       </c>
       <c r="D236" t="s">
         <v>113</v>
@@ -7415,7 +7415,7 @@
         <v>6</v>
       </c>
       <c r="H236">
-        <v>1036552477.649676</v>
+        <v>904787332.1857345</v>
       </c>
       <c r="I236">
         <v>0</v>
@@ -7433,7 +7433,7 @@
         <v>17748900625</v>
       </c>
       <c r="N236">
-        <v>4176844324.595036</v>
+        <v>3915302873.830781</v>
       </c>
     </row>
     <row r="237" spans="1:14">
@@ -7493,7 +7493,7 @@
         <v>0</v>
       </c>
       <c r="G239">
-        <v>736</v>
+        <v>721</v>
       </c>
     </row>
     <row r="240" spans="1:14">
@@ -8206,7 +8206,7 @@
         <v>129</v>
       </c>
       <c r="G267">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="268" spans="1:14">
@@ -8227,7 +8227,7 @@
         <v>129</v>
       </c>
       <c r="G268">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="269" spans="1:14">
@@ -8248,7 +8248,7 @@
         <v>130</v>
       </c>
       <c r="G269">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="270" spans="1:14">
@@ -8257,7 +8257,7 @@
         <v>106</v>
       </c>
       <c r="C270">
-        <v>0.8383233532934131</v>
+        <v>0.8203592814371258</v>
       </c>
       <c r="D270" t="s">
         <v>113</v>
@@ -8266,7 +8266,7 @@
         <v>2</v>
       </c>
       <c r="H270">
-        <v>1314733379.62963</v>
+        <v>1183260041.666667</v>
       </c>
       <c r="I270">
         <v>0</v>
@@ -8284,7 +8284,7 @@
         <v>17748900625</v>
       </c>
       <c r="N270">
-        <v>4736831148.585345</v>
+        <v>4503040417.341418</v>
       </c>
     </row>
     <row r="271" spans="1:14">
@@ -8344,7 +8344,7 @@
         <v>0</v>
       </c>
       <c r="G273">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="274" spans="1:14">
@@ -9908,7 +9908,7 @@
         <v>129</v>
       </c>
       <c r="G335">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="336" spans="1:13">
@@ -9925,8 +9925,8 @@
       <c r="E336">
         <v>12</v>
       </c>
-      <c r="F336" t="s">
-        <v>129</v>
+      <c r="F336">
+        <v>0</v>
       </c>
       <c r="G336">
         <v>17</v>
@@ -9950,7 +9950,7 @@
         <v>130</v>
       </c>
       <c r="G337">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="338" spans="1:14">
@@ -9959,7 +9959,7 @@
         <v>106</v>
       </c>
       <c r="C338">
-        <v>0.6666666666666666</v>
+        <v>0.6458333333333334</v>
       </c>
       <c r="D338" t="s">
         <v>113</v>
@@ -10046,7 +10046,7 @@
         <v>0</v>
       </c>
       <c r="G341">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="342" spans="1:14">
@@ -10759,7 +10759,7 @@
         <v>129</v>
       </c>
       <c r="G369">
-        <v>3201</v>
+        <v>3058</v>
       </c>
     </row>
     <row r="370" spans="1:14">
@@ -10780,7 +10780,7 @@
         <v>129</v>
       </c>
       <c r="G370">
-        <v>1716</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="371" spans="1:14">
@@ -10801,7 +10801,7 @@
         <v>130</v>
       </c>
       <c r="G371">
-        <v>1782</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="372" spans="1:14">
@@ -10810,7 +10810,7 @@
         <v>106</v>
       </c>
       <c r="C372">
-        <v>0.7675550405561993</v>
+        <v>0.7344148319814601</v>
       </c>
       <c r="D372" t="s">
         <v>113</v>
@@ -10897,7 +10897,7 @@
         <v>0</v>
       </c>
       <c r="G375">
-        <v>3317</v>
+        <v>3174</v>
       </c>
     </row>
     <row r="376" spans="1:14">
@@ -14972,7 +14972,7 @@
         <v>129</v>
       </c>
       <c r="G539">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="540" spans="1:14">
@@ -14993,7 +14993,7 @@
         <v>129</v>
       </c>
       <c r="G540">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="541" spans="1:14">
@@ -15014,7 +15014,7 @@
         <v>130</v>
       </c>
       <c r="G541">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="542" spans="1:14">
@@ -15023,7 +15023,7 @@
         <v>106</v>
       </c>
       <c r="C542">
-        <v>0.8829787234042553</v>
+        <v>0.8617021276595744</v>
       </c>
       <c r="D542" t="s">
         <v>113</v>
@@ -15110,7 +15110,7 @@
         <v>0</v>
       </c>
       <c r="G545">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="546" spans="1:14">
@@ -15823,7 +15823,7 @@
         <v>129</v>
       </c>
       <c r="G573">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="574" spans="1:14">
@@ -15844,7 +15844,7 @@
         <v>129</v>
       </c>
       <c r="G574">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="575" spans="1:14">
@@ -15865,7 +15865,7 @@
         <v>130</v>
       </c>
       <c r="G575">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="576" spans="1:14">
@@ -15874,7 +15874,7 @@
         <v>106</v>
       </c>
       <c r="C576">
-        <v>0.8451327433628318</v>
+        <v>0.8362831858407079</v>
       </c>
       <c r="D576" t="s">
         <v>113</v>
@@ -15961,7 +15961,7 @@
         <v>0</v>
       </c>
       <c r="G579">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="580" spans="1:14">
@@ -19167,7 +19167,7 @@
         <v>129</v>
       </c>
       <c r="G709">
-        <v>548</v>
+        <v>522</v>
       </c>
     </row>
     <row r="710" spans="1:14">
@@ -19188,7 +19188,7 @@
         <v>129</v>
       </c>
       <c r="G710">
-        <v>275</v>
+        <v>250</v>
       </c>
     </row>
     <row r="711" spans="1:14">
@@ -19209,7 +19209,7 @@
         <v>130</v>
       </c>
       <c r="G711">
-        <v>285</v>
+        <v>260</v>
       </c>
     </row>
     <row r="712" spans="1:14">
@@ -19218,7 +19218,7 @@
         <v>106</v>
       </c>
       <c r="C712">
-        <v>0.8282387190684134</v>
+        <v>0.7903930131004366</v>
       </c>
       <c r="D712" t="s">
         <v>113</v>
@@ -19305,7 +19305,7 @@
         <v>0</v>
       </c>
       <c r="G715">
-        <v>569</v>
+        <v>543</v>
       </c>
     </row>
     <row r="716" spans="1:14">
@@ -20018,7 +20018,7 @@
         <v>129</v>
       </c>
       <c r="G743">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="744" spans="1:14">
@@ -20039,7 +20039,7 @@
         <v>129</v>
       </c>
       <c r="G744">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="745" spans="1:14">
@@ -20060,7 +20060,7 @@
         <v>130</v>
       </c>
       <c r="G745">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="746" spans="1:14">
@@ -20069,7 +20069,7 @@
         <v>106</v>
       </c>
       <c r="C746">
-        <v>0.8913043478260869</v>
+        <v>0.8478260869565217</v>
       </c>
       <c r="D746" t="s">
         <v>113</v>
@@ -20078,7 +20078,7 @@
         <v>2</v>
       </c>
       <c r="H746">
-        <v>1183260041.666667</v>
+        <v>845185744.0476191</v>
       </c>
       <c r="I746">
         <v>0</v>
@@ -20090,13 +20090,13 @@
         <v>0</v>
       </c>
       <c r="L746">
-        <v>2958150104.166667</v>
+        <v>1479075052.083333</v>
       </c>
       <c r="M746">
         <v>2958150104.166667</v>
       </c>
       <c r="N746">
-        <v>1620245540.53834</v>
+        <v>1443429451.224481</v>
       </c>
     </row>
     <row r="747" spans="1:14">
@@ -20156,7 +20156,7 @@
         <v>0</v>
       </c>
       <c r="G749">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="750" spans="1:14">
@@ -21699,7 +21699,7 @@
         <v>129</v>
       </c>
       <c r="G811">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="812" spans="1:14">
@@ -21720,7 +21720,7 @@
         <v>129</v>
       </c>
       <c r="G812">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="813" spans="1:14">
@@ -21741,7 +21741,7 @@
         <v>130</v>
       </c>
       <c r="G813">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="814" spans="1:14">
@@ -21750,7 +21750,7 @@
         <v>106</v>
       </c>
       <c r="C814">
-        <v>0.8412698412698413</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="D814" t="s">
         <v>113</v>
@@ -21759,7 +21759,7 @@
         <v>3</v>
       </c>
       <c r="H814">
-        <v>135121.6059027778</v>
+        <v>128687.2437169312</v>
       </c>
       <c r="I814">
         <v>0</v>
@@ -21777,7 +21777,7 @@
         <v>8104520.833333334</v>
       </c>
       <c r="N814">
-        <v>1046283.128698476</v>
+        <v>1021068.068405191</v>
       </c>
     </row>
     <row r="815" spans="1:14">
@@ -21837,7 +21837,7 @@
         <v>0</v>
       </c>
       <c r="G817">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="818" spans="1:14">
@@ -22550,7 +22550,7 @@
         <v>129</v>
       </c>
       <c r="G845">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="846" spans="1:14">
@@ -22571,7 +22571,7 @@
         <v>129</v>
       </c>
       <c r="G846">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="847" spans="1:14">
@@ -22592,7 +22592,7 @@
         <v>130</v>
       </c>
       <c r="G847">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="848" spans="1:14">
@@ -22601,7 +22601,7 @@
         <v>106</v>
       </c>
       <c r="C848">
-        <v>0.896551724137931</v>
+        <v>0.8620689655172413</v>
       </c>
       <c r="D848" t="s">
         <v>113</v>
@@ -22688,7 +22688,7 @@
         <v>0</v>
       </c>
       <c r="G851">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="852" spans="1:14">
@@ -23401,7 +23401,7 @@
         <v>129</v>
       </c>
       <c r="G879">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="880" spans="1:13">
@@ -23422,7 +23422,7 @@
         <v>129</v>
       </c>
       <c r="G880">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="881" spans="1:14">
@@ -23443,7 +23443,7 @@
         <v>130</v>
       </c>
       <c r="G881">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="882" spans="1:14">
@@ -23452,7 +23452,7 @@
         <v>106</v>
       </c>
       <c r="C882">
-        <v>0.9122137404580153</v>
+        <v>0.8969465648854962</v>
       </c>
       <c r="D882" t="s">
         <v>113</v>
@@ -23539,7 +23539,7 @@
         <v>0</v>
       </c>
       <c r="G885">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="886" spans="1:14">
@@ -24252,7 +24252,7 @@
         <v>129</v>
       </c>
       <c r="G913">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="914" spans="1:14">
@@ -24273,7 +24273,7 @@
         <v>129</v>
       </c>
       <c r="G914">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="915" spans="1:14">
@@ -24294,7 +24294,7 @@
         <v>130</v>
       </c>
       <c r="G915">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="916" spans="1:14">
@@ -24303,7 +24303,7 @@
         <v>106</v>
       </c>
       <c r="C916">
-        <v>0.8129496402877698</v>
+        <v>0.7877697841726619</v>
       </c>
       <c r="D916" t="s">
         <v>113</v>
@@ -24390,7 +24390,7 @@
         <v>0</v>
       </c>
       <c r="G919">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="920" spans="1:14">
@@ -25933,7 +25933,7 @@
         <v>129</v>
       </c>
       <c r="G981">
-        <v>751</v>
+        <v>705</v>
       </c>
     </row>
     <row r="982" spans="1:14">
@@ -25954,7 +25954,7 @@
         <v>129</v>
       </c>
       <c r="G982">
-        <v>433</v>
+        <v>388</v>
       </c>
     </row>
     <row r="983" spans="1:14">
@@ -25975,7 +25975,7 @@
         <v>130</v>
       </c>
       <c r="G983">
-        <v>516</v>
+        <v>471</v>
       </c>
     </row>
     <row r="984" spans="1:14">
@@ -25984,7 +25984,7 @@
         <v>106</v>
       </c>
       <c r="C984">
-        <v>0.8215417106652587</v>
+        <v>0.7729672650475184</v>
       </c>
       <c r="D984" t="s">
         <v>113</v>
@@ -26071,7 +26071,7 @@
         <v>0</v>
       </c>
       <c r="G987">
-        <v>781</v>
+        <v>735</v>
       </c>
     </row>
     <row r="988" spans="1:14">
@@ -27635,7 +27635,7 @@
         <v>129</v>
       </c>
       <c r="G1049">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="1050" spans="1:14">
@@ -27652,8 +27652,8 @@
       <c r="E1050">
         <v>7</v>
       </c>
-      <c r="F1050" t="s">
-        <v>129</v>
+      <c r="F1050">
+        <v>0</v>
       </c>
       <c r="G1050">
         <v>12</v>
@@ -27673,8 +27673,8 @@
       <c r="E1051">
         <v>4</v>
       </c>
-      <c r="F1051" t="s">
-        <v>130</v>
+      <c r="F1051">
+        <v>0</v>
       </c>
       <c r="G1051">
         <v>12</v>
@@ -27686,7 +27686,7 @@
         <v>106</v>
       </c>
       <c r="C1052">
-        <v>0.6875</v>
+        <v>0.625</v>
       </c>
       <c r="D1052" t="s">
         <v>113</v>
@@ -27773,7 +27773,7 @@
         <v>0</v>
       </c>
       <c r="G1055">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="1056" spans="1:14">
@@ -30185,7 +30185,7 @@
         <v>129</v>
       </c>
       <c r="G1151">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="1152" spans="1:13">
@@ -30206,7 +30206,7 @@
         <v>129</v>
       </c>
       <c r="G1152">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="1153" spans="1:14">
@@ -30227,7 +30227,7 @@
         <v>130</v>
       </c>
       <c r="G1153">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="1154" spans="1:14">
@@ -30236,7 +30236,7 @@
         <v>106</v>
       </c>
       <c r="C1154">
-        <v>0.8536585365853658</v>
+        <v>0.8292682926829268</v>
       </c>
       <c r="D1154" t="s">
         <v>113</v>
@@ -30323,7 +30323,7 @@
         <v>0</v>
       </c>
       <c r="G1157">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="1158" spans="1:14">
@@ -32702,7 +32702,7 @@
         <v>129</v>
       </c>
       <c r="G1253">
-        <v>542</v>
+        <v>530</v>
       </c>
     </row>
     <row r="1254" spans="1:14">
@@ -32717,13 +32717,13 @@
         <v>111</v>
       </c>
       <c r="E1254">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F1254" t="s">
         <v>129</v>
       </c>
       <c r="G1254">
-        <v>281</v>
+        <v>270</v>
       </c>
     </row>
     <row r="1255" spans="1:14">
@@ -32744,7 +32744,7 @@
         <v>130</v>
       </c>
       <c r="G1255">
-        <v>312</v>
+        <v>301</v>
       </c>
     </row>
     <row r="1256" spans="1:14">
@@ -32753,7 +32753,7 @@
         <v>106</v>
       </c>
       <c r="C1256">
-        <v>0.8984848484848484</v>
+        <v>0.8803030303030303</v>
       </c>
       <c r="D1256" t="s">
         <v>113</v>
@@ -32762,7 +32762,7 @@
         <v>2</v>
       </c>
       <c r="H1256">
-        <v>120962.9975124378</v>
+        <v>102588.8713080169</v>
       </c>
       <c r="I1256">
         <v>0</v>
@@ -32780,7 +32780,7 @@
         <v>8104520.833333334</v>
       </c>
       <c r="N1256">
-        <v>990124.8069824333</v>
+        <v>911829.8332386231</v>
       </c>
     </row>
     <row r="1257" spans="1:14">
@@ -32840,7 +32840,7 @@
         <v>0</v>
       </c>
       <c r="G1259">
-        <v>594</v>
+        <v>582</v>
       </c>
     </row>
     <row r="1260" spans="1:14">
@@ -33553,7 +33553,7 @@
         <v>129</v>
       </c>
       <c r="G1287">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="1288" spans="1:14">
@@ -33574,7 +33574,7 @@
         <v>129</v>
       </c>
       <c r="G1288">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1289" spans="1:14">
@@ -33595,7 +33595,7 @@
         <v>130</v>
       </c>
       <c r="G1289">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="1290" spans="1:14">
@@ -33604,7 +33604,7 @@
         <v>106</v>
       </c>
       <c r="C1290">
-        <v>0.7647058823529411</v>
+        <v>0.7058823529411765</v>
       </c>
       <c r="D1290" t="s">
         <v>113</v>
@@ -33691,7 +33691,7 @@
         <v>0</v>
       </c>
       <c r="G1293">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="1294" spans="1:14">
@@ -34404,7 +34404,7 @@
         <v>129</v>
       </c>
       <c r="G1321">
-        <v>756</v>
+        <v>713</v>
       </c>
     </row>
     <row r="1322" spans="1:14">
@@ -34425,7 +34425,7 @@
         <v>129</v>
       </c>
       <c r="G1322">
-        <v>512</v>
+        <v>468</v>
       </c>
     </row>
     <row r="1323" spans="1:14">
@@ -34446,7 +34446,7 @@
         <v>130</v>
       </c>
       <c r="G1323">
-        <v>544</v>
+        <v>500</v>
       </c>
     </row>
     <row r="1324" spans="1:14">
@@ -34455,7 +34455,7 @@
         <v>106</v>
       </c>
       <c r="C1324">
-        <v>0.7568555758683729</v>
+        <v>0.7157221206581352</v>
       </c>
       <c r="D1324" t="s">
         <v>113</v>
@@ -34464,7 +34464,7 @@
         <v>3</v>
       </c>
       <c r="H1324">
-        <v>914043.7030075188</v>
+        <v>781786.575562701</v>
       </c>
       <c r="I1324">
         <v>0</v>
@@ -34482,7 +34482,7 @@
         <v>97254250</v>
       </c>
       <c r="N1324">
-        <v>8914507.7822366</v>
+        <v>8248420.26013595</v>
       </c>
     </row>
     <row r="1325" spans="1:14">
@@ -34542,7 +34542,7 @@
         <v>0</v>
       </c>
       <c r="G1327">
-        <v>832</v>
+        <v>787</v>
       </c>
     </row>
     <row r="1328" spans="1:14">
@@ -35255,7 +35255,7 @@
         <v>129</v>
       </c>
       <c r="G1355">
-        <v>6089</v>
+        <v>5877</v>
       </c>
     </row>
     <row r="1356" spans="1:14">
@@ -35276,7 +35276,7 @@
         <v>129</v>
       </c>
       <c r="G1356">
-        <v>3095</v>
+        <v>2888</v>
       </c>
     </row>
     <row r="1357" spans="1:14">
@@ -35297,7 +35297,7 @@
         <v>130</v>
       </c>
       <c r="G1357">
-        <v>3436</v>
+        <v>3228</v>
       </c>
     </row>
     <row r="1358" spans="1:14">
@@ -35306,7 +35306,7 @@
         <v>106</v>
       </c>
       <c r="C1358">
-        <v>0.8616822429906542</v>
+        <v>0.8331108144192256</v>
       </c>
       <c r="D1358" t="s">
         <v>113</v>
@@ -35315,7 +35315,7 @@
         <v>8</v>
       </c>
       <c r="H1358">
-        <v>171646510.7841659</v>
+        <v>142260628.1379167</v>
       </c>
       <c r="I1358">
         <v>0</v>
@@ -35333,7 +35333,7 @@
         <v>17748900625</v>
       </c>
       <c r="N1358">
-        <v>1736153533.194135</v>
+        <v>1581759688.54137</v>
       </c>
     </row>
     <row r="1359" spans="1:14">
@@ -35393,7 +35393,7 @@
         <v>0</v>
       </c>
       <c r="G1361">
-        <v>6494</v>
+        <v>6280</v>
       </c>
     </row>
     <row r="1362" spans="1:14">
@@ -36106,7 +36106,7 @@
         <v>129</v>
       </c>
       <c r="G1389">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="1390" spans="1:14">
@@ -36127,7 +36127,7 @@
         <v>129</v>
       </c>
       <c r="G1390">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="1391" spans="1:14">
@@ -36148,7 +36148,7 @@
         <v>130</v>
       </c>
       <c r="G1391">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="1392" spans="1:14">
@@ -36157,7 +36157,7 @@
         <v>106</v>
       </c>
       <c r="C1392">
-        <v>0.9310344827586207</v>
+        <v>0.896551724137931</v>
       </c>
       <c r="D1392" t="s">
         <v>113</v>
@@ -36244,7 +36244,7 @@
         <v>0</v>
       </c>
       <c r="G1395">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="1396" spans="1:14">
@@ -36957,7 +36957,7 @@
         <v>129</v>
       </c>
       <c r="G1423">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="1424" spans="1:13">
@@ -36974,11 +36974,11 @@
       <c r="E1424">
         <v>3</v>
       </c>
-      <c r="F1424" t="s">
-        <v>129</v>
+      <c r="F1424">
+        <v>0</v>
       </c>
       <c r="G1424">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="1425" spans="1:14">
@@ -36995,11 +36995,11 @@
       <c r="E1425">
         <v>3</v>
       </c>
-      <c r="F1425" t="s">
-        <v>130</v>
+      <c r="F1425">
+        <v>0</v>
       </c>
       <c r="G1425">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="1426" spans="1:14">
@@ -37008,7 +37008,7 @@
         <v>106</v>
       </c>
       <c r="C1426">
-        <v>0.5714285714285714</v>
+        <v>0.5</v>
       </c>
       <c r="D1426" t="s">
         <v>113</v>
@@ -37095,7 +37095,7 @@
         <v>0</v>
       </c>
       <c r="G1429">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="1430" spans="1:14">
@@ -38638,7 +38638,7 @@
         <v>129</v>
       </c>
       <c r="G1491">
-        <v>346</v>
+        <v>329</v>
       </c>
     </row>
     <row r="1492" spans="1:14">
@@ -38653,13 +38653,13 @@
         <v>111</v>
       </c>
       <c r="E1492">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F1492" t="s">
         <v>129</v>
       </c>
       <c r="G1492">
-        <v>181</v>
+        <v>167</v>
       </c>
     </row>
     <row r="1493" spans="1:14">
@@ -38680,7 +38680,7 @@
         <v>130</v>
       </c>
       <c r="G1493">
-        <v>200</v>
+        <v>186</v>
       </c>
     </row>
     <row r="1494" spans="1:14">
@@ -38689,7 +38689,7 @@
         <v>106</v>
       </c>
       <c r="C1494">
-        <v>0.8881118881118881</v>
+        <v>0.8484848484848485</v>
       </c>
       <c r="D1494" t="s">
         <v>113</v>
@@ -38776,7 +38776,7 @@
         <v>0</v>
       </c>
       <c r="G1497">
-        <v>381</v>
+        <v>364</v>
       </c>
     </row>
     <row r="1498" spans="1:14">
@@ -40340,7 +40340,7 @@
         <v>129</v>
       </c>
       <c r="G1559">
-        <v>561</v>
+        <v>551</v>
       </c>
     </row>
     <row r="1560" spans="1:14">
@@ -40355,13 +40355,13 @@
         <v>111</v>
       </c>
       <c r="E1560">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F1560" t="s">
         <v>129</v>
       </c>
       <c r="G1560">
-        <v>266</v>
+        <v>258</v>
       </c>
     </row>
     <row r="1561" spans="1:14">
@@ -40382,7 +40382,7 @@
         <v>130</v>
       </c>
       <c r="G1561">
-        <v>327</v>
+        <v>317</v>
       </c>
     </row>
     <row r="1562" spans="1:14">
@@ -40391,7 +40391,7 @@
         <v>106</v>
       </c>
       <c r="C1562">
-        <v>0.9169184290030211</v>
+        <v>0.9018126888217523</v>
       </c>
       <c r="D1562" t="s">
         <v>113</v>
@@ -40400,7 +40400,7 @@
         <v>2</v>
       </c>
       <c r="H1562">
-        <v>107569094.6969697</v>
+        <v>91020003.20512821</v>
       </c>
       <c r="I1562">
         <v>0</v>
@@ -40418,7 +40418,7 @@
         <v>2958150104.166667</v>
       </c>
       <c r="N1562">
-        <v>558849562.6797472</v>
+        <v>514824035.6792662</v>
       </c>
     </row>
     <row r="1563" spans="1:14">
@@ -40478,7 +40478,7 @@
         <v>0</v>
       </c>
       <c r="G1565">
-        <v>610</v>
+        <v>600</v>
       </c>
     </row>
     <row r="1566" spans="1:14">
@@ -41191,7 +41191,7 @@
         <v>129</v>
       </c>
       <c r="G1593">
-        <v>436</v>
+        <v>420</v>
       </c>
     </row>
     <row r="1594" spans="1:14">
@@ -41212,7 +41212,7 @@
         <v>129</v>
       </c>
       <c r="G1594">
-        <v>262</v>
+        <v>246</v>
       </c>
     </row>
     <row r="1595" spans="1:14">
@@ -41233,7 +41233,7 @@
         <v>130</v>
       </c>
       <c r="G1595">
-        <v>269</v>
+        <v>253</v>
       </c>
     </row>
     <row r="1596" spans="1:14">
@@ -41242,7 +41242,7 @@
         <v>106</v>
       </c>
       <c r="C1596">
-        <v>0.9201451905626135</v>
+        <v>0.8911070780399274</v>
       </c>
       <c r="D1596" t="s">
         <v>113</v>
@@ -41251,7 +41251,7 @@
         <v>3</v>
       </c>
       <c r="H1596">
-        <v>405594428.9772727</v>
+        <v>297435914.5833333</v>
       </c>
       <c r="I1596">
         <v>0</v>
@@ -41269,7 +41269,7 @@
         <v>17748900625</v>
       </c>
       <c r="N1596">
-        <v>2675426076.020335</v>
+        <v>2291177312.618682</v>
       </c>
     </row>
     <row r="1597" spans="1:14">
@@ -41329,7 +41329,7 @@
         <v>0</v>
       </c>
       <c r="G1599">
-        <v>511</v>
+        <v>495</v>
       </c>
     </row>
     <row r="1600" spans="1:14">
@@ -42872,7 +42872,7 @@
         <v>129</v>
       </c>
       <c r="G1661">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="1662" spans="1:14">
@@ -42893,7 +42893,7 @@
         <v>129</v>
       </c>
       <c r="G1662">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="1663" spans="1:14">
@@ -42914,7 +42914,7 @@
         <v>130</v>
       </c>
       <c r="G1663">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="1664" spans="1:14">
@@ -42923,7 +42923,7 @@
         <v>106</v>
       </c>
       <c r="C1664">
-        <v>0.8942307692307693</v>
+        <v>0.8798076923076923</v>
       </c>
       <c r="D1664" t="s">
         <v>113</v>
@@ -42932,7 +42932,7 @@
         <v>3</v>
       </c>
       <c r="H1664">
-        <v>1615746744.318182</v>
+        <v>1421857135</v>
       </c>
       <c r="I1664">
         <v>0</v>
@@ -42950,7 +42950,7 @@
         <v>17748900625</v>
       </c>
       <c r="N1664">
-        <v>5221819084.01793</v>
+        <v>4913872236.590238</v>
       </c>
     </row>
     <row r="1665" spans="1:14">
@@ -43010,7 +43010,7 @@
         <v>0</v>
       </c>
       <c r="G1667">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="1668" spans="1:14">
@@ -43723,7 +43723,7 @@
         <v>129</v>
       </c>
       <c r="G1695">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="1696" spans="1:13">
@@ -43744,7 +43744,7 @@
         <v>129</v>
       </c>
       <c r="G1696">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="1697" spans="1:14">
@@ -43765,7 +43765,7 @@
         <v>130</v>
       </c>
       <c r="G1697">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="1698" spans="1:14">
@@ -43774,7 +43774,7 @@
         <v>106</v>
       </c>
       <c r="C1698">
-        <v>0.8627450980392157</v>
+        <v>0.8431372549019608</v>
       </c>
       <c r="D1698" t="s">
         <v>113</v>
@@ -43861,7 +43861,7 @@
         <v>0</v>
       </c>
       <c r="G1701">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1702" spans="1:14">
@@ -44574,7 +44574,7 @@
         <v>129</v>
       </c>
       <c r="G1729">
-        <v>684</v>
+        <v>648</v>
       </c>
     </row>
     <row r="1730" spans="1:14">
@@ -44595,7 +44595,7 @@
         <v>129</v>
       </c>
       <c r="G1730">
-        <v>335</v>
+        <v>300</v>
       </c>
     </row>
     <row r="1731" spans="1:14">
@@ -44616,7 +44616,7 @@
         <v>130</v>
       </c>
       <c r="G1731">
-        <v>375</v>
+        <v>339</v>
       </c>
     </row>
     <row r="1732" spans="1:14">
@@ -44625,7 +44625,7 @@
         <v>106</v>
       </c>
       <c r="C1732">
-        <v>0.8265424912689173</v>
+        <v>0.7846332945285215</v>
       </c>
       <c r="D1732" t="s">
         <v>113</v>
@@ -44634,7 +44634,7 @@
         <v>2</v>
       </c>
       <c r="H1732">
-        <v>119120138.4228188</v>
+        <v>95940003.37837838</v>
       </c>
       <c r="I1732">
         <v>0</v>
@@ -44652,7 +44652,7 @@
         <v>17748900625</v>
       </c>
       <c r="N1732">
-        <v>1454046594.612035</v>
+        <v>1304925126.558992</v>
       </c>
     </row>
     <row r="1733" spans="1:14">
@@ -44712,7 +44712,7 @@
         <v>0</v>
       </c>
       <c r="G1735">
-        <v>714</v>
+        <v>678</v>
       </c>
     </row>
     <row r="1736" spans="1:14">
@@ -45419,13 +45419,13 @@
         <v>111</v>
       </c>
       <c r="E1763">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F1763" t="s">
         <v>129</v>
       </c>
       <c r="G1763">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="1764" spans="1:14">
@@ -45440,7 +45440,7 @@
         <v>111</v>
       </c>
       <c r="E1764">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F1764">
         <v>1</v>
@@ -45461,7 +45461,7 @@
         <v>111</v>
       </c>
       <c r="E1765">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1765">
         <v>3</v>
@@ -45476,12 +45476,33 @@
         <v>106</v>
       </c>
       <c r="C1766">
-        <v>1</v>
+        <v>0.9473684210526315</v>
       </c>
       <c r="D1766" t="s">
         <v>113</v>
       </c>
       <c r="E1766">
+        <v>1</v>
+      </c>
+      <c r="H1766">
+        <v>0</v>
+      </c>
+      <c r="I1766">
+        <v>0</v>
+      </c>
+      <c r="J1766">
+        <v>0</v>
+      </c>
+      <c r="K1766">
+        <v>0</v>
+      </c>
+      <c r="L1766">
+        <v>0</v>
+      </c>
+      <c r="M1766">
+        <v>0</v>
+      </c>
+      <c r="N1766">
         <v>0</v>
       </c>
     </row>
@@ -45536,13 +45557,13 @@
         <v>0</v>
       </c>
       <c r="E1769">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F1769" t="b">
         <v>0</v>
       </c>
       <c r="G1769">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="1770" spans="1:14">
@@ -46255,7 +46276,7 @@
         <v>129</v>
       </c>
       <c r="G1797">
-        <v>793</v>
+        <v>778</v>
       </c>
     </row>
     <row r="1798" spans="1:14">
@@ -46276,7 +46297,7 @@
         <v>129</v>
       </c>
       <c r="G1798">
-        <v>414</v>
+        <v>399</v>
       </c>
     </row>
     <row r="1799" spans="1:14">
@@ -46297,7 +46318,7 @@
         <v>130</v>
       </c>
       <c r="G1799">
-        <v>458</v>
+        <v>443</v>
       </c>
     </row>
     <row r="1800" spans="1:14">
@@ -46306,7 +46327,7 @@
         <v>106</v>
       </c>
       <c r="C1800">
-        <v>0.8756319514661274</v>
+        <v>0.8604651162790697</v>
       </c>
       <c r="D1800" t="s">
         <v>113</v>
@@ -46393,7 +46414,7 @@
         <v>0</v>
       </c>
       <c r="G1803">
-        <v>871</v>
+        <v>856</v>
       </c>
     </row>
     <row r="1804" spans="1:14">
@@ -48772,7 +48793,7 @@
         <v>129</v>
       </c>
       <c r="G1899">
-        <v>609</v>
+        <v>599</v>
       </c>
     </row>
     <row r="1900" spans="1:14">
@@ -48787,13 +48808,13 @@
         <v>111</v>
       </c>
       <c r="E1900">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F1900" t="s">
         <v>129</v>
       </c>
       <c r="G1900">
-        <v>326</v>
+        <v>317</v>
       </c>
     </row>
     <row r="1901" spans="1:14">
@@ -48814,7 +48835,7 @@
         <v>130</v>
       </c>
       <c r="G1901">
-        <v>369</v>
+        <v>360</v>
       </c>
     </row>
     <row r="1902" spans="1:14">
@@ -48823,7 +48844,7 @@
         <v>106</v>
       </c>
       <c r="C1902">
-        <v>0.8919270833333334</v>
+        <v>0.87890625</v>
       </c>
       <c r="D1902" t="s">
         <v>113</v>
@@ -48832,7 +48853,7 @@
         <v>2</v>
       </c>
       <c r="H1902">
-        <v>641526528.6144578</v>
+        <v>572545181.4516129</v>
       </c>
       <c r="I1902">
         <v>0</v>
@@ -48850,7 +48871,7 @@
         <v>17748900625</v>
       </c>
       <c r="N1902">
-        <v>3332967710.714081</v>
+        <v>3152956303.565258</v>
       </c>
     </row>
     <row r="1903" spans="1:14">
@@ -48910,7 +48931,7 @@
         <v>0</v>
       </c>
       <c r="G1905">
-        <v>689</v>
+        <v>679</v>
       </c>
     </row>
     <row r="1906" spans="1:14">
@@ -50474,7 +50495,7 @@
         <v>129</v>
       </c>
       <c r="G1967">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="1968" spans="1:13">
@@ -50495,7 +50516,7 @@
         <v>129</v>
       </c>
       <c r="G1968">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="1969" spans="1:14">
@@ -50516,7 +50537,7 @@
         <v>130</v>
       </c>
       <c r="G1969">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="1970" spans="1:14">
@@ -50525,7 +50546,7 @@
         <v>106</v>
       </c>
       <c r="C1970">
-        <v>0.9130434782608695</v>
+        <v>0.8869565217391304</v>
       </c>
       <c r="D1970" t="s">
         <v>113</v>
@@ -50534,7 +50555,7 @@
         <v>2</v>
       </c>
       <c r="H1970">
-        <v>3647034.375</v>
+        <v>2805411.057692308</v>
       </c>
       <c r="I1970">
         <v>0</v>
@@ -50552,7 +50573,7 @@
         <v>36470343.75</v>
       </c>
       <c r="N1970">
-        <v>11532935.32992865</v>
+        <v>10115053.41726328</v>
       </c>
     </row>
     <row r="1971" spans="1:14">
@@ -50612,7 +50633,7 @@
         <v>0</v>
       </c>
       <c r="G1973">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="1974" spans="1:14">
@@ -51325,7 +51346,7 @@
         <v>129</v>
       </c>
       <c r="G2001">
-        <v>238</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2002" spans="1:14">
@@ -51346,7 +51367,7 @@
         <v>129</v>
       </c>
       <c r="G2002">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2003" spans="1:14">
@@ -51367,7 +51388,7 @@
         <v>130</v>
       </c>
       <c r="G2003">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2004" spans="1:14">
@@ -51376,7 +51397,7 @@
         <v>106</v>
       </c>
       <c r="C2004">
-        <v>0.7887788778877888</v>
+        <v>0.759075907590759</v>
       </c>
       <c r="D2004" t="s">
         <v>113</v>
@@ -51385,7 +51406,7 @@
         <v>3</v>
       </c>
       <c r="H2004">
-        <v>3165.828450520833</v>
+        <v>2775.520833333333</v>
       </c>
       <c r="I2004">
         <v>0</v>
@@ -51403,7 +51424,7 @@
         <v>199837.5</v>
       </c>
       <c r="N2004">
-        <v>24975.36567201293</v>
+        <v>23385.81048406948</v>
       </c>
     </row>
     <row r="2005" spans="1:14">
@@ -51463,7 +51484,7 @@
         <v>0</v>
       </c>
       <c r="G2007">
-        <v>242</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2008" spans="1:14">
@@ -52176,7 +52197,7 @@
         <v>129</v>
       </c>
       <c r="G2035">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2036" spans="1:14">
@@ -52197,7 +52218,7 @@
         <v>129</v>
       </c>
       <c r="G2036">
-        <v>104</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2037" spans="1:14">
@@ -52218,7 +52239,7 @@
         <v>130</v>
       </c>
       <c r="G2037">
-        <v>116</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2038" spans="1:14">
@@ -52227,7 +52248,7 @@
         <v>106</v>
       </c>
       <c r="C2038">
-        <v>0.7695652173913043</v>
+        <v>0.7173913043478261</v>
       </c>
       <c r="D2038" t="s">
         <v>113</v>
@@ -52236,7 +52257,7 @@
         <v>2</v>
       </c>
       <c r="H2038">
-        <v>917492.9245283019</v>
+        <v>748109.6153846154</v>
       </c>
       <c r="I2038">
         <v>0</v>
@@ -52254,7 +52275,7 @@
         <v>48627125</v>
       </c>
       <c r="N2038">
-        <v>6679449.313203395</v>
+        <v>6031452.543211264</v>
       </c>
     </row>
     <row r="2039" spans="1:14">
@@ -52314,7 +52335,7 @@
         <v>0</v>
       </c>
       <c r="G2041">
-        <v>178</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2042" spans="1:14">
@@ -53027,7 +53048,7 @@
         <v>129</v>
       </c>
       <c r="G2069">
-        <v>1019</v>
+        <v>987</v>
       </c>
     </row>
     <row r="2070" spans="1:14">
@@ -53048,7 +53069,7 @@
         <v>129</v>
       </c>
       <c r="G2070">
-        <v>541</v>
+        <v>511</v>
       </c>
     </row>
     <row r="2071" spans="1:14">
@@ -53069,7 +53090,7 @@
         <v>130</v>
       </c>
       <c r="G2071">
-        <v>585</v>
+        <v>553</v>
       </c>
     </row>
     <row r="2072" spans="1:14">
@@ -53078,7 +53099,7 @@
         <v>106</v>
       </c>
       <c r="C2072">
-        <v>0.8730548730548731</v>
+        <v>0.8468468468468469</v>
       </c>
       <c r="D2072" t="s">
         <v>113</v>
@@ -53165,7 +53186,7 @@
         <v>0</v>
       </c>
       <c r="G2075">
-        <v>1066</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="2076" spans="1:14">
@@ -54729,7 +54750,7 @@
         <v>129</v>
       </c>
       <c r="G2137">
-        <v>537</v>
+        <v>516</v>
       </c>
     </row>
     <row r="2138" spans="1:14">
@@ -54750,7 +54771,7 @@
         <v>129</v>
       </c>
       <c r="G2138">
-        <v>244</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2139" spans="1:14">
@@ -54771,7 +54792,7 @@
         <v>130</v>
       </c>
       <c r="G2139">
-        <v>303</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2140" spans="1:14">
@@ -54780,7 +54801,7 @@
         <v>106</v>
       </c>
       <c r="C2140">
-        <v>0.7954866008462623</v>
+        <v>0.765867418899859</v>
       </c>
       <c r="D2140" t="s">
         <v>113</v>
@@ -54867,7 +54888,7 @@
         <v>0</v>
       </c>
       <c r="G2143">
-        <v>565</v>
+        <v>544</v>
       </c>
     </row>
     <row r="2144" spans="1:14">
@@ -55580,7 +55601,7 @@
         <v>129</v>
       </c>
       <c r="G2171">
-        <v>1058</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="2172" spans="1:14">
@@ -55601,7 +55622,7 @@
         <v>129</v>
       </c>
       <c r="G2172">
-        <v>572</v>
+        <v>522</v>
       </c>
     </row>
     <row r="2173" spans="1:14">
@@ -55622,7 +55643,7 @@
         <v>130</v>
       </c>
       <c r="G2173">
-        <v>642</v>
+        <v>592</v>
       </c>
     </row>
     <row r="2174" spans="1:14">
@@ -55631,7 +55652,7 @@
         <v>106</v>
       </c>
       <c r="C2174">
-        <v>0.7037267080745342</v>
+        <v>0.6726708074534161</v>
       </c>
       <c r="D2174" t="s">
         <v>113</v>
@@ -55640,7 +55661,7 @@
         <v>5</v>
       </c>
       <c r="H2174">
-        <v>155481069.4881202</v>
+        <v>140729544.868754</v>
       </c>
       <c r="I2174">
         <v>0</v>
@@ -55658,7 +55679,7 @@
         <v>17748900625</v>
       </c>
       <c r="N2174">
-        <v>1625255262.841662</v>
+        <v>1546753291.43367</v>
       </c>
     </row>
     <row r="2175" spans="1:14">
@@ -55718,7 +55739,7 @@
         <v>0</v>
       </c>
       <c r="G2177">
-        <v>1146</v>
+        <v>1096</v>
       </c>
     </row>
   </sheetData>

</xml_diff>